<commit_message>
updated mapping from RBN to FN
</commit_message>
<xml_diff>
--- a/mapping_to_fn/Mapping.xlsx
+++ b/mapping_to_fn/Mapping.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
   <si>
     <t>RBN feature set</t>
   </si>
@@ -32,6 +32,9 @@
     <t>Intentionally_act</t>
   </si>
   <si>
+    <t>English FrameNet frames</t>
+  </si>
+  <si>
     <t>high in the tree</t>
   </si>
   <si>
@@ -62,9 +65,15 @@
     <t>subcat of Intentially_act</t>
   </si>
   <si>
+    <t>Children</t>
+  </si>
+  <si>
     <t>...</t>
   </si>
   <si>
+    <t>mvmt1</t>
+  </si>
+  <si>
     <t>excprod2</t>
   </si>
   <si>
@@ -80,6 +89,9 @@
     <t>excprod3</t>
   </si>
   <si>
+    <t>Motion,Operate_vehicle_scenario,Traversing</t>
+  </si>
+  <si>
     <t>mvmnt1</t>
   </si>
   <si>
@@ -92,22 +104,28 @@
     <t>mvmnt2</t>
   </si>
   <si>
-    <t>English FrameNet frames</t>
+    <t>mvmnt3</t>
+  </si>
+  <si>
+    <t>Cogn1</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Cogn1Fluidic_motion,Mass_motion,Motion_directional,Motion_noise,Self_motion,Cause_to_land,Getting_vehicle_underway,Operate_vehicle,Traversing</t>
+  </si>
+  <si>
+    <t>ook: prmvmt</t>
   </si>
   <si>
     <t>mvmt2</t>
   </si>
   <si>
-    <t>Motion,Intentionally_act</t>
-  </si>
-  <si>
-    <t>mvmnt3</t>
-  </si>
-  <si>
-    <t>Cogn1</t>
-  </si>
-  <si>
-    <t>Statement</t>
+    <t>mvmt3</t>
   </si>
   <si>
     <t>Affirm_or_deny, Complaining, Predicting, Reading_aloud, Recording, Reveal_secret, Telling</t>
@@ -119,17 +137,89 @@
     <t>Communication_manner, Communication_noise, Communication_response, Gesture, Reassuring, Summarizing</t>
   </si>
   <si>
+    <t>prmvmt1</t>
+  </si>
+  <si>
     <t>make_noise</t>
   </si>
   <si>
     <t>Cogn2</t>
+  </si>
+  <si>
+    <t>prmvmt2</t>
+  </si>
+  <si>
+    <t>prmvmt3</t>
+  </si>
+  <si>
+    <t>echprod2</t>
+  </si>
+  <si>
+    <t>Transfer,Giving,Receiving</t>
+  </si>
+  <si>
+    <t>Commerce_goods-transfer, Commerce_money-transfer,Giving,Receiving</t>
+  </si>
+  <si>
+    <t>echprod3</t>
+  </si>
+  <si>
+    <t>cognt1</t>
+  </si>
+  <si>
+    <t>Perception</t>
+  </si>
+  <si>
+    <t>Becoming_aware,Give_impression,Perception_active,Perception_experience,Sensation</t>
+  </si>
+  <si>
+    <t>Affirm_or_deny,Complaining,Predicting,Reading_aloud,Recording,Reveal_secret, Telling</t>
+  </si>
+  <si>
+    <t>Communication_manner,Communication_noise,Communication_response,Gesture,Reassuring,Summarizing</t>
+  </si>
+  <si>
+    <t>Make_noise</t>
+  </si>
+  <si>
+    <t>Judgement</t>
+  </si>
+  <si>
+    <t>Judgement_communication</t>
+  </si>
+  <si>
+    <t>Bragging,Judgment_direct_address</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+  <si>
+    <t>cognt2</t>
+  </si>
+  <si>
+    <t>cognt3</t>
+  </si>
+  <si>
+    <t>probably all frames with a cognizant or perceptor</t>
+  </si>
+  <si>
+    <t>location1</t>
+  </si>
+  <si>
+    <t>Being_attached,Being_detached</t>
+  </si>
+  <si>
+    <t>Being_attached,Being_detached,Being_located,Presence,Visiting</t>
+  </si>
+  <si>
+    <t>location2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -140,17 +230,32 @@
     </font>
     <font/>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -172,8 +277,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -202,8 +319,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.43"/>
-    <col customWidth="1" min="2" max="2" width="24.86"/>
-    <col customWidth="1" min="3" max="3" width="22.29"/>
+    <col customWidth="1" min="2" max="2" width="45.0"/>
+    <col customWidth="1" min="3" max="3" width="45.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -229,138 +346,137 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>27</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -378,9 +494,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.57"/>
-    <col customWidth="1" min="2" max="2" width="41.86"/>
-    <col customWidth="1" min="3" max="3" width="16.57"/>
+    <col customWidth="1" min="1" max="1" width="23.86"/>
+    <col customWidth="1" min="2" max="2" width="47.71"/>
+    <col customWidth="1" min="3" max="3" width="22.86"/>
+    <col customWidth="1" min="4" max="4" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -388,22 +505,475 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36">
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38">
+      <c r="C38" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>